<commit_message>
Conferência LN - PEC
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_PEC.xlsx
+++ b/Documentação/Planilhas/Conferencia_PEC.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="stg_pec_cab" sheetId="104" r:id="rId1"/>
-    <sheet name="Plan1" sheetId="102" r:id="rId2"/>
+    <sheet name="stg_pec_det" sheetId="105" r:id="rId2"/>
+    <sheet name="Plan1" sheetId="102" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="357">
   <si>
     <t>1</t>
   </si>
@@ -131,30 +132,12 @@
     <t>1403</t>
   </si>
   <si>
-    <t>R20000001</t>
-  </si>
-  <si>
-    <t>R20000011</t>
-  </si>
-  <si>
     <t>000000017</t>
   </si>
   <si>
-    <t>R20000019</t>
-  </si>
-  <si>
-    <t>R20000020</t>
-  </si>
-  <si>
-    <t>R20000021</t>
-  </si>
-  <si>
     <t>N00004</t>
   </si>
   <si>
-    <t>R00000009</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -296,9 +279,6 @@
     <t>100-Não aplicável</t>
   </si>
   <si>
-    <t>R20000106</t>
-  </si>
-  <si>
     <t>R20000345</t>
   </si>
   <si>
@@ -854,9 +834,6 @@
     <t>No menu "Specific", selecionar "Histórico de Ordem". Novamente no menu "Specific", desmarcar a opção "Última Entrada por Ordem". Pegar a data mais antiga apresentada para a ordem desejada, cujo status seja igual a "Aprovado"</t>
   </si>
   <si>
-    <t>o campo "rcd_utc" não é apresentado nas telas do LN. Refete a data de alteração dos registros na tabela dtpur401</t>
-  </si>
-  <si>
     <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar uma linha e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Dados Fiscais", pegar a informação do CFOP</t>
   </si>
   <si>
@@ -864,6 +841,252 @@
   </si>
   <si>
     <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar uma linha e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Despesas (Valores Rateados)", pegar a informação do Seguro [somar o valor de todos os itens da ordem]</t>
+  </si>
+  <si>
+    <t>Selecionar a ordem desejada e com o botão direito do mouse, escolher "Text" e em seguida "Texto do Cabeçalho"</t>
+  </si>
+  <si>
+    <t>Não tem em ordem de compra. Mandei um e-mail para o Patrick perguntando se podemos eliminá-lo</t>
+  </si>
+  <si>
+    <t>Segundo o Fábio, não faz sentido termos no CAB, pois aqui não tem item. Mandei um e-mail ao Patrick perguntando se podemos eliminá-lo</t>
+  </si>
+  <si>
+    <t>stg_pec_det</t>
+  </si>
+  <si>
+    <t>NR_ITEM_NFR_REFERENCIA</t>
+  </si>
+  <si>
+    <t>CD_ITEM</t>
+  </si>
+  <si>
+    <t>CD_UNIDADE_MEDIDA</t>
+  </si>
+  <si>
+    <t>QT_PEDIDO</t>
+  </si>
+  <si>
+    <t>VL_UNITARIO_ORIGINAL_ITEM</t>
+  </si>
+  <si>
+    <t>VL_UNITARIO_ATUAL_ITEM</t>
+  </si>
+  <si>
+    <t>QT_ENTREGUE</t>
+  </si>
+  <si>
+    <t>DT_ENTREGA</t>
+  </si>
+  <si>
+    <t>QT_ENTREGUE_EXCESSO</t>
+  </si>
+  <si>
+    <t>QT_LIQUIDADA</t>
+  </si>
+  <si>
+    <t>QT_CANCELADA</t>
+  </si>
+  <si>
+    <t>CD_STATUS_ITEM</t>
+  </si>
+  <si>
+    <t>DS_OBSERVACAO_ITEM</t>
+  </si>
+  <si>
+    <t>VL_PERCENTUAL_DESCONTO</t>
+  </si>
+  <si>
+    <t>CD_ITEM_KIT</t>
+  </si>
+  <si>
+    <t>900000258</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>2.0000</t>
+  </si>
+  <si>
+    <t>1019.4000</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>2222.30</t>
+  </si>
+  <si>
+    <t>900000259</t>
+  </si>
+  <si>
+    <t>3.0000</t>
+  </si>
+  <si>
+    <t>1349.4000</t>
+  </si>
+  <si>
+    <t>4412.53</t>
+  </si>
+  <si>
+    <t>900000260</t>
+  </si>
+  <si>
+    <t>10.0000</t>
+  </si>
+  <si>
+    <t>359.4000</t>
+  </si>
+  <si>
+    <t>3917.46</t>
+  </si>
+  <si>
+    <t>C10000004</t>
+  </si>
+  <si>
+    <t>900000295</t>
+  </si>
+  <si>
+    <t>126.2100</t>
+  </si>
+  <si>
+    <t>2013-10-19 12:57:39.000</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>126.21</t>
+  </si>
+  <si>
+    <t>2403</t>
+  </si>
+  <si>
+    <t>900000296</t>
+  </si>
+  <si>
+    <t>217.5200</t>
+  </si>
+  <si>
+    <t>217.52</t>
+  </si>
+  <si>
+    <t>C10000005</t>
+  </si>
+  <si>
+    <t>107.EC-WB150FVDWBR</t>
+  </si>
+  <si>
+    <t>2013-10-31 10:40:00.000</t>
+  </si>
+  <si>
+    <t>100000.00</t>
+  </si>
+  <si>
+    <t>1657240</t>
+  </si>
+  <si>
+    <t>90NB0051-M02180</t>
+  </si>
+  <si>
+    <t>900000376</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna Ordem de Compra</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Linha da Ordem", pegar a informação da coluna "Linha"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Linha da Ordem", pegar a segunda informação da coluna "Item"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Linha da Ordem", pegar a primeira  informação da coluna "Quantidade Ordenada" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Linha da Ordem", pegar a  segunda informação da coluna "Quantidade Ordenada" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Linha da Ordem", pegar a  informação da coluna "Preço" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Ir para a sessão "tdipu0101m000" e informar o CD_ITEM desejado na segunda coluna do "Item". Pegar a informação da coluna "Preço de Compra"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior Recebimentos", pegar a  informação da coluna "Quantidade Recebida" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem desejada. Na aba inferior "Monitor", aba "Parceiros de Negócios" pegar a informação da coluna "Data planejada de Recebimento Atual" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Se QT_ENTREGUE &gt; QT_PEDIDO, faremos o cálculo [QT_ENTREGUE - QT_PEDIDO]. Caso contrário, retorna zero</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Linha da Ordem", verificar se a coluna "Cancelado" está selecionada para o item desejado. Se tiver, retornará "C". Se não estiver selecionada.....</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Recebimentos", pegar a  informação da coluna "Quantidade Rejeitada" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da Ordem de Compra desejada. Na aba inferior "Recebimentos", pegar a  informação da coluna "Quantidade Aprovada" de cada item desejado</t>
+  </si>
+  <si>
+    <t>Ir para a aba inferior "Recebimentos" e verificar se a coluna "Rec. Final" está ticada para o item desejado. Se tiver, retornará "L", caso não esteja ticada, retornará "A"</t>
+  </si>
+  <si>
+    <t>C20001859</t>
+  </si>
+  <si>
+    <t>900001653</t>
+  </si>
+  <si>
+    <t>2000.0000</t>
+  </si>
+  <si>
+    <t>2014-06-18 15:43:00.000</t>
+  </si>
+  <si>
+    <t>BARUERI</t>
+  </si>
+  <si>
+    <t>2000.00</t>
+  </si>
+  <si>
+    <t>2933</t>
+  </si>
+  <si>
+    <t>o campo "rcd_utc" não é apresentado nas telas do LN. Refete a data de alteração dos registros na tabela tdpur401</t>
+  </si>
+  <si>
+    <t>não tem em compras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informar o CD_ITEM na sessão "tcibd0501m000", na segunda lacuna da coluna "Item" e pedir o seu detalhamento. Na aba superior " Dados Item Nova", seção "Características", pegar a informação de "Observação" </t>
+  </si>
+  <si>
+    <t>Desconto de Linha</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar a linha do item desejado e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Despesas (Valores Rateados)", pegar a informação do Frete</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar a linha do item desejado e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Despesas (Valores Rateados)", pegar a informação do Seguro</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar a linha do item desejado e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Valores", pegar a informação do "Valor Total da Linha"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar uma linha e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Valores", pegar a informação do "Valor Total da Linha" [somar o valor de todos os itens existente no pedido]</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", marcar a linha do item desejado e no menu "Specific", selecionar "Linhas da Previsão de Impostos".  Na seção "Dados Fiscais", pegar a informação do "CFOP"</t>
+  </si>
+  <si>
+    <t>Fazer o detalhamento da ordem desejada. Na aba inferior "Linhas da Ordem", fazer o detalhamento do item desejado. Na aba superior "Recebimento", pegar a informação de "Item Kit" [no final da tela]</t>
+  </si>
+  <si>
+    <t>2014-06-24 10:40:18.000</t>
   </si>
 </sst>
 </file>
@@ -902,7 +1125,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -939,6 +1162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -967,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -991,21 +1220,6 @@
     <xf numFmtId="49" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1021,6 +1235,30 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,8 +1268,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFFFFCC"/>
+      <color rgb="FFFA7E7E"/>
       <color rgb="FF99FFCC"/>
-      <color rgb="FFFA7E7E"/>
       <color rgb="FFCCECFF"/>
       <color rgb="FFFF5050"/>
     </mruColors>
@@ -1329,9 +1567,7 @@
   </sheetPr>
   <dimension ref="A2:AQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AE6" sqref="AE6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -1349,24 +1585,24 @@
     <col min="12" max="12" width="21.5703125" style="1" customWidth="1"/>
     <col min="13" max="13" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.140625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="25.140625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="30" style="1" customWidth="1"/>
-    <col min="18" max="18" width="24.42578125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="38.85546875" style="1" customWidth="1"/>
-    <col min="20" max="20" width="31.42578125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="39.5703125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="42.85546875" style="1" customWidth="1"/>
-    <col min="23" max="23" width="40.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="29.5703125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="33.140625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="36.7109375" style="1" customWidth="1"/>
-    <col min="27" max="27" width="37.140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="36.85546875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="25.85546875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="25" style="1" customWidth="1"/>
-    <col min="31" max="31" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="25.85546875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="30.5703125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="25.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30" style="1" customWidth="1"/>
+    <col min="19" max="19" width="24.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="38.85546875" style="1" customWidth="1"/>
+    <col min="21" max="21" width="31.42578125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="39.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="42.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="40.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="40.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="29.5703125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="36.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="37.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="36.85546875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="25" style="1" customWidth="1"/>
+    <col min="32" max="32" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="34.42578125" style="1" customWidth="1"/>
     <col min="34" max="34" width="31.42578125" style="1" customWidth="1"/>
     <col min="35" max="35" width="29" style="1" customWidth="1"/>
@@ -1382,435 +1618,435 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:43" ht="21">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="10"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="21">
+      <c r="A3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" s="13" customFormat="1" ht="18" customHeight="1">
+      <c r="A6" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="K6" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="O6" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="P6" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="R6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="T6" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="U6" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="V6" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="W6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="X6" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y6" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="Z6" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA6" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB6" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="AC6" s="19" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="3" spans="1:43" ht="21">
-      <c r="A3" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="7" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:43" s="18" customFormat="1" ht="18" customHeight="1">
-      <c r="A6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="L6" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="N6" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="O6" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="P6" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q6" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="R6" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="S6" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="T6" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="U6" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="V6" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="W6" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="X6" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y6" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="Z6" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="AA6" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="AB6" s="15" t="s">
+      <c r="AD6" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE6" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF6" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="AC6" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="AD6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE6" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="AF6" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="AG6" s="15" t="s">
+      <c r="AG6" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="AH6" s="16"/>
-      <c r="AI6" s="16"/>
-      <c r="AJ6" s="16"/>
-      <c r="AK6" s="17"/>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
-      <c r="AO6" s="16"/>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="16"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
     </row>
     <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="N7" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="U7" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="14" t="s">
+      <c r="V7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="W7" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="X7" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="Z7" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA7" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB7" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="AC7" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" s="14" t="s">
+      <c r="AD7" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P7" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q7" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="R7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="S7" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="T7" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="U7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="V7" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="W7" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="X7" s="14" t="s">
-        <v>156</v>
-      </c>
-      <c r="Y7" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z7" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="AA7" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB7" s="14" t="s">
-        <v>149</v>
-      </c>
-      <c r="AC7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AF7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AF7" s="1" t="s">
-        <v>152</v>
-      </c>
       <c r="AG7" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>225</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="D8" s="14" t="s">
+      <c r="B8" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G8" s="14" t="s">
+      <c r="F8" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="M8" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="N8" s="14" t="s">
+      <c r="M8" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="N8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="O8" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="P8" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q8" s="14" t="s">
+      <c r="O8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P8" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="R8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="R8" s="14" t="s">
+      <c r="S8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="S8" s="14" t="s">
+      <c r="T8" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="T8" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="U8" s="14" t="s">
+      <c r="U8" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="V8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="V8" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="W8" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="X8" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="Y8" s="14" t="s">
+      <c r="W8" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z8" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AA8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Z8" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="AA8" s="14" t="s">
+      <c r="AB8" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AB8" s="14" t="s">
+      <c r="AD8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AE8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AF8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AF8" s="1" t="s">
-        <v>229</v>
-      </c>
       <c r="AG8" s="1" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="P9" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q9" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="S9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="W9" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="X9" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y9" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="AD9" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF9" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="D9" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O9" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="Q9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="R9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="S9" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="T9" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="U9" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="V9" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="W9" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="X9" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y9" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z9" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AA9" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AB9" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC9" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="AD9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE9" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF9" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="AG9" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:43">
@@ -1818,10 +2054,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>36</v>
@@ -1830,7 +2066,7 @@
         <v>29</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>0</v>
@@ -1839,79 +2075,79 @@
         <v>15</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="P10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB10" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="Q10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="AB10" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="AC10" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AD10" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AE10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE10" s="1" t="s">
+      <c r="AF10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AF10" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="AG10" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -1919,19 +2155,19 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>0</v>
@@ -1940,7 +2176,7 @@
         <v>15</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>1</v>
@@ -1952,7 +2188,7 @@
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>1</v>
@@ -1961,58 +2197,58 @@
         <v>10</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>154</v>
+        <v>10</v>
       </c>
       <c r="Q11" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="R11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S11" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="T11" s="1" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="U11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="V11" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="W11" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
       <c r="Y11" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z11" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z11" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA11" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="AB11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC11" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AE11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AF11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AF11" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="AG11" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -2020,19 +2256,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>0</v>
@@ -2041,7 +2277,7 @@
         <v>15</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>1</v>
@@ -2053,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>1</v>
@@ -2062,58 +2298,58 @@
         <v>10</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="Q12" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S12" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="T12" s="1" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>173</v>
+        <v>124</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
       <c r="AC12" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AD12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD12" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE12" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF12" s="1" t="s">
-        <v>175</v>
+      <c r="AF12" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:43">
@@ -2121,19 +2357,19 @@
         <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>0</v>
@@ -2142,7 +2378,7 @@
         <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>1</v>
@@ -2154,7 +2390,7 @@
         <v>0</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>1</v>
@@ -2163,58 +2399,58 @@
         <v>10</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S13" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="T13" s="1" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>131</v>
+        <v>176</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>181</v>
+        <v>124</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="AC13" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD13" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>183</v>
+      <c r="AF13" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:43">
@@ -2222,19 +2458,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>1</v>
@@ -2243,7 +2479,7 @@
         <v>15</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>1</v>
@@ -2255,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>1</v>
@@ -2264,58 +2500,58 @@
         <v>10</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>137</v>
+        <v>10</v>
       </c>
       <c r="Q14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S14" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="T14" s="1" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="U14" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="V14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V14" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="W14" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>189</v>
+        <v>127</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>131</v>
+        <v>183</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="AA14" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AC14" s="1" t="s">
+      <c r="AE14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD14" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE14" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF14" s="1" t="s">
-        <v>190</v>
+      <c r="AF14" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:43">
@@ -2323,19 +2559,19 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>0</v>
@@ -2344,7 +2580,7 @@
         <v>15</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>1</v>
@@ -2356,67 +2592,67 @@
         <v>0</v>
       </c>
       <c r="M15" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Q15" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S15" s="1" t="s">
+      <c r="T15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T15" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="U15" s="1" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>196</v>
+        <v>127</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>193</v>
+        <v>124</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="AC15" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE15" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE15" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF15" s="1" t="s">
-        <v>175</v>
+      <c r="AF15" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="AG15" s="1" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:43">
@@ -2424,19 +2660,19 @@
         <v>2</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>0</v>
@@ -2445,7 +2681,7 @@
         <v>15</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>1</v>
@@ -2457,708 +2693,759 @@
         <v>0</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="Q16" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="T16" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T16" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="U16" s="1" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="X16" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF16" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:33" ht="11.25" customHeight="1"/>
+    <row r="20" spans="1:33" ht="11.25" customHeight="1">
+      <c r="A20" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>262</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="L20" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="M20" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="O20" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="P20" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q20" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="R20" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="S20" s="15" t="s">
+        <v>249</v>
+      </c>
+      <c r="T20" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="U20" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="V20" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="W20" s="14" t="s">
+        <v>273</v>
+      </c>
+      <c r="X20" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="Y20" s="14" t="s">
+        <v>353</v>
+      </c>
+      <c r="Z20" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="AA20" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="AB20" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="AC20" s="14" t="s">
+        <v>271</v>
+      </c>
+      <c r="AD20" s="14" t="s">
+        <v>270</v>
+      </c>
+      <c r="AE20" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF20" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="AG20" s="14" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="14"/>
+      <c r="X21" s="14"/>
+      <c r="Y21" s="14"/>
+      <c r="Z21" s="14"/>
+      <c r="AA21" s="14"/>
+      <c r="AB21" s="14"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="14"/>
+      <c r="AE21" s="15"/>
+      <c r="AF21" s="15"/>
+      <c r="AG21" s="14"/>
+    </row>
+    <row r="22" spans="1:33">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="14"/>
+      <c r="X22" s="14"/>
+      <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="14"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="14"/>
+      <c r="AE22" s="15"/>
+      <c r="AF22" s="15"/>
+      <c r="AG22" s="14"/>
+    </row>
+    <row r="23" spans="1:33">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="14"/>
+      <c r="X23" s="14"/>
+      <c r="Y23" s="14"/>
+      <c r="Z23" s="14"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="14"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="14"/>
+      <c r="AE23" s="15"/>
+      <c r="AF23" s="15"/>
+      <c r="AG23" s="14"/>
+    </row>
+    <row r="24" spans="1:33">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="15"/>
+      <c r="AF24" s="15"/>
+      <c r="AG24" s="14"/>
+    </row>
+    <row r="26" spans="1:33" ht="11.25" customHeight="1">
+      <c r="E26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="K26" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33">
+      <c r="E27" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="R27" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33">
+      <c r="E28" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="Y16" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Z16" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="AA16" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="AB16" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AC16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="AE16" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AF16" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AG16" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:33">
-      <c r="AG19" s="12" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="20" spans="1:33" ht="11.25" customHeight="1">
-      <c r="A20" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="I28" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="R28" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33">
+      <c r="E29" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="R29" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33">
+      <c r="E30" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="K30" s="18"/>
+      <c r="R30" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33">
+      <c r="E31" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K31" s="18"/>
+      <c r="R31" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33">
+      <c r="E32" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>230</v>
-      </c>
-      <c r="H20" s="9" t="s">
+      <c r="I32" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="I20" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="K20" s="9" t="s">
+      <c r="K32" s="18"/>
+      <c r="R32" s="9" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="33" spans="5:18">
+      <c r="E33" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="L20" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="M20" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="N20" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="O20" s="9" t="s">
+      <c r="I33" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="P20" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q20" s="9" t="s">
-        <v>255</v>
-      </c>
-      <c r="R20" s="9" t="s">
+      <c r="R33" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="S20" s="12" t="s">
-        <v>272</v>
-      </c>
-      <c r="T20" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="U20" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="V20" s="12" t="s">
-        <v>281</v>
-      </c>
-      <c r="W20" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="X20" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="Y20" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="Z20" s="12" t="s">
-        <v>276</v>
-      </c>
-      <c r="AA20" s="12" t="s">
-        <v>278</v>
-      </c>
-      <c r="AB20" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="AG20" s="12"/>
-    </row>
-    <row r="21" spans="1:33">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="12"/>
-      <c r="V21" s="12"/>
-      <c r="W21" s="12"/>
-      <c r="X21" s="12"/>
-      <c r="Y21" s="12"/>
-      <c r="Z21" s="12"/>
-      <c r="AA21" s="12"/>
-      <c r="AB21" s="12"/>
-      <c r="AG21" s="12"/>
-    </row>
-    <row r="22" spans="1:33">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="12"/>
-      <c r="T22" s="12"/>
-      <c r="U22" s="12"/>
-      <c r="V22" s="12"/>
-      <c r="W22" s="12"/>
-      <c r="X22" s="12"/>
-      <c r="Y22" s="12"/>
-      <c r="Z22" s="12"/>
-      <c r="AA22" s="12"/>
-      <c r="AB22" s="12"/>
-      <c r="AG22" s="12"/>
-    </row>
-    <row r="23" spans="1:33">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="12"/>
-      <c r="Z23" s="12"/>
-      <c r="AA23" s="12"/>
-      <c r="AB23" s="12"/>
-      <c r="AG23" s="12"/>
-    </row>
-    <row r="24" spans="1:33">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="12"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="12"/>
-      <c r="V24" s="12"/>
-      <c r="W24" s="12"/>
-      <c r="X24" s="12"/>
-      <c r="Y24" s="12"/>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="12"/>
-      <c r="AB24" s="12"/>
-    </row>
-    <row r="26" spans="1:33" ht="11.25" customHeight="1">
-      <c r="E26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>206</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="Q26" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="S26" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="27" spans="1:33">
-      <c r="E27" s="14" t="s">
+    </row>
+    <row r="34" spans="5:18">
+      <c r="E34" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="F27" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="I27" s="14" t="s">
+      <c r="I34" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="Q27" s="14" t="s">
+      <c r="R34" s="9" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
-      <c r="E28" s="14" t="s">
+    <row r="35" spans="5:18">
+      <c r="E35" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F28" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="I35" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="Q28" s="14" t="s">
+      <c r="R35" s="9" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
-      <c r="E29" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>209</v>
-      </c>
-      <c r="I29" s="14" t="s">
+    <row r="36" spans="5:18">
+      <c r="I36" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="Q29" s="14" t="s">
+      <c r="R36" s="9" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
-      <c r="E30" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="I30" s="14" t="s">
+    <row r="37" spans="5:18">
+      <c r="I37" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="K30" s="13"/>
-      <c r="Q30" s="14" t="s">
+      <c r="R37" s="9" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
-      <c r="E31" s="14" t="s">
-        <v>216</v>
-      </c>
-      <c r="I31" s="14" t="s">
+    <row r="38" spans="5:18">
+      <c r="I38" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="K31" s="13"/>
-      <c r="Q31" s="14" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="32" spans="1:33">
-      <c r="E32" s="14" t="s">
-        <v>217</v>
-      </c>
-      <c r="I32" s="14" t="s">
+      <c r="R38" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="5:18">
+      <c r="I39" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="K32" s="13"/>
-      <c r="Q32" s="14" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="33" spans="5:17">
-      <c r="E33" s="14" t="s">
-        <v>218</v>
-      </c>
-      <c r="I33" s="14" t="s">
+      <c r="R39" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="5:18">
+      <c r="I40" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="Q33" s="14" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="34" spans="5:17">
-      <c r="E34" s="14" t="s">
-        <v>219</v>
-      </c>
-      <c r="I34" s="14" t="s">
+      <c r="R40" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="5:18">
+      <c r="I41" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="Q34" s="14" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="35" spans="5:17">
-      <c r="E35" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="I35" s="14" t="s">
+      <c r="R41" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="5:18">
+      <c r="I42" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="Q35" s="14" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="36" spans="5:17">
-      <c r="I36" s="14" t="s">
+      <c r="R42" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="5:18">
+      <c r="I43" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="Q36" s="14" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="37" spans="5:17">
-      <c r="I37" s="14" t="s">
+      <c r="R43" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="5:18">
+      <c r="I44" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="Q37" s="14" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="38" spans="5:17">
-      <c r="I38" s="14" t="s">
+      <c r="R44" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="5:18">
+      <c r="I45" s="9" t="s">
         <v>244</v>
       </c>
-      <c r="Q38" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="5:17">
-      <c r="I39" s="14" t="s">
+      <c r="R45" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="5:18">
+      <c r="I46" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="Q39" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="5:17">
-      <c r="I40" s="14" t="s">
+      <c r="R46" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="5:18">
+      <c r="I47" s="9" t="s">
         <v>246</v>
       </c>
-      <c r="Q40" s="14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="41" spans="5:17">
-      <c r="I41" s="14" t="s">
+      <c r="R47" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="5:18">
+      <c r="I48" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="Q41" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="42" spans="5:17">
-      <c r="I42" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="Q42" s="14" t="s">
+      <c r="R48" s="9" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="43" spans="5:17">
-      <c r="I43" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="Q43" s="14" t="s">
+    <row r="49" spans="18:18">
+      <c r="R49" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="44" spans="5:17">
-      <c r="I44" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q44" s="14" t="s">
+    <row r="50" spans="18:18">
+      <c r="R50" s="9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="5:17">
-      <c r="I45" s="14" t="s">
-        <v>251</v>
-      </c>
-      <c r="Q45" s="14" t="s">
+    <row r="51" spans="18:18">
+      <c r="R51" s="9" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="5:17">
-      <c r="I46" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="Q46" s="14" t="s">
+    <row r="52" spans="18:18">
+      <c r="R52" s="9" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="5:17">
-      <c r="I47" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="Q47" s="14" t="s">
+    <row r="53" spans="18:18">
+      <c r="R53" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="48" spans="5:17">
-      <c r="I48" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q48" s="14" t="s">
+    <row r="54" spans="18:18">
+      <c r="R54" s="9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="17:17">
-      <c r="Q49" s="14" t="s">
+    <row r="55" spans="18:18">
+      <c r="R55" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="17:17">
-      <c r="Q50" s="14" t="s">
+    <row r="56" spans="18:18">
+      <c r="R56" s="9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="17:17">
-      <c r="Q51" s="14" t="s">
+    <row r="57" spans="18:18">
+      <c r="R57" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="17:17">
-      <c r="Q52" s="14" t="s">
+    <row r="58" spans="18:18">
+      <c r="R58" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="17:17">
-      <c r="Q53" s="14" t="s">
+    <row r="59" spans="18:18">
+      <c r="R59" s="9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="54" spans="17:17">
-      <c r="Q54" s="14" t="s">
+    <row r="60" spans="18:18">
+      <c r="R60" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="17:17">
-      <c r="Q55" s="14" t="s">
+    <row r="61" spans="18:18">
+      <c r="R61" s="9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="56" spans="17:17">
-      <c r="Q56" s="14" t="s">
+    <row r="62" spans="18:18">
+      <c r="R62" s="9" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="17:17">
-      <c r="Q57" s="14" t="s">
+    <row r="63" spans="18:18">
+      <c r="R63" s="9" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="17:17">
-      <c r="Q58" s="14" t="s">
+    <row r="64" spans="18:18">
+      <c r="R64" s="9" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="17:17">
-      <c r="Q59" s="14" t="s">
+    <row r="65" spans="18:18">
+      <c r="R65" s="9" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="17:17">
-      <c r="Q60" s="14" t="s">
+    <row r="66" spans="18:18">
+      <c r="R66" s="9" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="17:17">
-      <c r="Q61" s="14" t="s">
+    <row r="67" spans="18:18">
+      <c r="R67" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="17:17">
-      <c r="Q62" s="14" t="s">
+    <row r="68" spans="18:18">
+      <c r="R68" s="9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="17:17">
-      <c r="Q63" s="14" t="s">
+    <row r="69" spans="18:18">
+      <c r="R69" s="9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="17:17">
-      <c r="Q64" s="14" t="s">
+    <row r="70" spans="18:18">
+      <c r="R70" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="17:17">
-      <c r="Q65" s="14" t="s">
+    <row r="71" spans="18:18">
+      <c r="R71" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="17:17">
-      <c r="Q66" s="14" t="s">
+    <row r="72" spans="18:18">
+      <c r="R72" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="17:17">
-      <c r="Q67" s="14" t="s">
+    <row r="73" spans="18:18">
+      <c r="R73" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="17:17">
-      <c r="Q68" s="14" t="s">
+    <row r="74" spans="18:18">
+      <c r="R74" s="9" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="17:17">
-      <c r="Q69" s="14" t="s">
+    <row r="75" spans="18:18">
+      <c r="R75" s="9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="17:17">
-      <c r="Q70" s="14" t="s">
+    <row r="76" spans="18:18">
+      <c r="R76" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="17:17">
-      <c r="Q71" s="14" t="s">
+    <row r="77" spans="18:18">
+      <c r="R77" s="9" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="17:17">
-      <c r="Q72" s="14" t="s">
+    <row r="78" spans="18:18">
+      <c r="R78" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="17:17">
-      <c r="Q73" s="14" t="s">
+    <row r="79" spans="18:18">
+      <c r="R79" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="17:17">
-      <c r="Q74" s="14" t="s">
+    <row r="80" spans="18:18">
+      <c r="R80" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="17:17">
-      <c r="Q75" s="14" t="s">
+    <row r="81" spans="18:18">
+      <c r="R81" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="17:17">
-      <c r="Q76" s="14" t="s">
+    <row r="82" spans="18:18">
+      <c r="R82" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="17:17">
-      <c r="Q77" s="14" t="s">
+    <row r="83" spans="18:18">
+      <c r="R83" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="78" spans="17:17">
-      <c r="Q78" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="79" spans="17:17">
-      <c r="Q79" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="80" spans="17:17">
-      <c r="Q80" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="81" spans="17:17">
-      <c r="Q81" s="14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="82" spans="17:17">
-      <c r="Q82" s="14" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="83" spans="17:17">
-      <c r="Q83" s="14" t="s">
-        <v>92</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="37">
+    <mergeCell ref="AD20:AD24"/>
+    <mergeCell ref="AC20:AC24"/>
+    <mergeCell ref="O20:O24"/>
+    <mergeCell ref="AG20:AG24"/>
+    <mergeCell ref="Y20:Y24"/>
+    <mergeCell ref="AE20:AE24"/>
+    <mergeCell ref="AF20:AF24"/>
+    <mergeCell ref="K26:K32"/>
+    <mergeCell ref="M20:M24"/>
+    <mergeCell ref="N20:N24"/>
+    <mergeCell ref="J26:J29"/>
+    <mergeCell ref="P20:P24"/>
+    <mergeCell ref="Z20:Z24"/>
+    <mergeCell ref="AB20:AB24"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="L20:L24"/>
+    <mergeCell ref="K20:K24"/>
+    <mergeCell ref="Q20:Q24"/>
+    <mergeCell ref="S20:S24"/>
+    <mergeCell ref="R20:R24"/>
+    <mergeCell ref="T20:T24"/>
     <mergeCell ref="U20:U24"/>
+    <mergeCell ref="AA20:AA24"/>
     <mergeCell ref="V20:V24"/>
     <mergeCell ref="W20:W24"/>
+    <mergeCell ref="X20:X24"/>
     <mergeCell ref="A20:A24"/>
     <mergeCell ref="B20:B24"/>
     <mergeCell ref="D20:D24"/>
@@ -3169,26 +3456,6 @@
     <mergeCell ref="H20:H24"/>
     <mergeCell ref="I20:I24"/>
     <mergeCell ref="J20:J24"/>
-    <mergeCell ref="X20:X24"/>
-    <mergeCell ref="Z20:Z24"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="L20:L24"/>
-    <mergeCell ref="K20:K24"/>
-    <mergeCell ref="K26:K32"/>
-    <mergeCell ref="M20:M24"/>
-    <mergeCell ref="N20:N24"/>
-    <mergeCell ref="J26:J29"/>
-    <mergeCell ref="O20:O24"/>
-    <mergeCell ref="P20:P24"/>
-    <mergeCell ref="R20:R24"/>
-    <mergeCell ref="Q20:Q24"/>
-    <mergeCell ref="S20:S24"/>
-    <mergeCell ref="T20:T24"/>
-    <mergeCell ref="Y20:Y24"/>
-    <mergeCell ref="AB20:AB24"/>
-    <mergeCell ref="AA20:AA24"/>
-    <mergeCell ref="AG19:AG23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3197,136 +3464,1258 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A2:AQ31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="26.7109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="28.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="30.140625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="25.140625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="30.140625" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30.85546875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="31.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="30" style="1" customWidth="1"/>
+    <col min="21" max="21" width="32.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="30.5703125" style="1" customWidth="1"/>
+    <col min="23" max="23" width="42.85546875" style="1" customWidth="1"/>
+    <col min="24" max="24" width="40.85546875" style="1" customWidth="1"/>
+    <col min="25" max="25" width="33.7109375" style="1" customWidth="1"/>
+    <col min="26" max="26" width="29.5703125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="33.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="36.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="37.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="36.85546875" style="1" customWidth="1"/>
+    <col min="31" max="31" width="25" style="1" customWidth="1"/>
+    <col min="32" max="32" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.42578125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="31.42578125" style="1" customWidth="1"/>
+    <col min="35" max="35" width="29" style="1" customWidth="1"/>
+    <col min="36" max="36" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="51.5703125" style="1" customWidth="1"/>
+    <col min="43" max="43" width="27.85546875" style="1" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:43" ht="21">
+      <c r="A2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43" ht="21">
+      <c r="A3" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:43">
+      <c r="P4" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="6" spans="1:43" s="13" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>291</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>288</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="N6" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>290</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="T6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="U6" s="20" t="s">
+        <v>293</v>
+      </c>
+      <c r="V6" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="W6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="X6" s="11"/>
+      <c r="Y6" s="11"/>
+      <c r="Z6" s="11"/>
+      <c r="AA6" s="11"/>
+      <c r="AB6" s="11"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="11"/>
+      <c r="AE6" s="11"/>
+      <c r="AF6" s="11"/>
+      <c r="AG6" s="11"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="11"/>
+      <c r="AJ6" s="11"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="11"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="11"/>
+      <c r="AP6" s="11"/>
+      <c r="AQ6" s="11"/>
+    </row>
+    <row r="7" spans="1:43">
+      <c r="A7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q7" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="S7" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="U7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W7" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:43">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O8" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:43">
+      <c r="A9" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="T9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W9" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:43">
+      <c r="A10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:43">
+      <c r="A11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="T11" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W11" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:43">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W12" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:43">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="W13" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:43">
+      <c r="A14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W14" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:43">
+      <c r="A15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W15" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:43">
+      <c r="A16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="N16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="O16" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q16" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="R16" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="S16" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="W16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="11.25" customHeight="1">
+      <c r="A19" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="L19" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="M19" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="Q19" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="R19" s="14" t="s">
+        <v>351</v>
+      </c>
+      <c r="S19" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="T19" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="U19" s="14" t="s">
+        <v>355</v>
+      </c>
+      <c r="V19" s="14" t="s">
+        <v>346</v>
+      </c>
+      <c r="W19" s="21" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="Q20" s="14"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="21"/>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="Q21" s="14"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="14"/>
+      <c r="V21" s="14"/>
+      <c r="W21" s="21"/>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="Q22" s="14"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="14"/>
+      <c r="T22" s="14"/>
+      <c r="U22" s="14"/>
+      <c r="V22" s="14"/>
+      <c r="W22" s="21"/>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="Q23" s="14"/>
+      <c r="R23" s="14"/>
+      <c r="S23" s="14"/>
+      <c r="T23" s="14"/>
+      <c r="U23" s="14"/>
+      <c r="V23" s="14"/>
+      <c r="W23" s="21"/>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="21"/>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="O26" s="15" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="O27" s="15"/>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="O28" s="15"/>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="O29" s="15"/>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="O30" s="15"/>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="O31" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="O26:O31"/>
+    <mergeCell ref="E19:E24"/>
+    <mergeCell ref="V19:V24"/>
+    <mergeCell ref="Q19:Q24"/>
+    <mergeCell ref="R19:R24"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="B19:B24"/>
+    <mergeCell ref="C19:C24"/>
+    <mergeCell ref="D19:D24"/>
+    <mergeCell ref="F19:F24"/>
+    <mergeCell ref="G19:G24"/>
+    <mergeCell ref="M19:M24"/>
+    <mergeCell ref="N19:N24"/>
+    <mergeCell ref="K19:K24"/>
+    <mergeCell ref="W19:W24"/>
+    <mergeCell ref="S19:S24"/>
+    <mergeCell ref="T19:T24"/>
+    <mergeCell ref="U19:U24"/>
+    <mergeCell ref="L19:L24"/>
+    <mergeCell ref="O19:O24"/>
+    <mergeCell ref="H19:H24"/>
+    <mergeCell ref="I19:I24"/>
+    <mergeCell ref="J19:J24"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="C3:M77"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F35"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M9" sqref="M3:M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="3" spans="3:13">
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
       <c r="F3" t="str">
         <f>CONCATENATE(C3,",")</f>
         <v>CD_CIA,</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>38</v>
+      <c r="K3" s="9" t="s">
+        <v>139</v>
       </c>
       <c r="M3" t="str">
         <f>CONCATENATE("'",K3,"',")</f>
-        <v>'R20000001',</v>
+        <v>'C10000003',</v>
       </c>
     </row>
     <row r="4" spans="3:13">
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4:F67" si="0">CONCATENATE(C4,",")</f>
         <v>NR_PEDIDO_COMPRA,</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>39</v>
+      <c r="K4" s="1" t="s">
+        <v>308</v>
       </c>
       <c r="M4" t="str">
         <f t="shared" ref="M4:M12" si="1">CONCATENATE("'",K4,"',")</f>
-        <v>'R20000011',</v>
+        <v>'C10000004',</v>
       </c>
     </row>
     <row r="5" spans="3:13">
-      <c r="C5" s="15" t="s">
-        <v>104</v>
+      <c r="C5" s="10" t="s">
+        <v>279</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>DT_EMISSAO_PEDIDO,</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>41</v>
+        <v>NR_ITEM_NFR_REFERENCIA,</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>318</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" si="1"/>
-        <v>'R20000019',</v>
+        <v>'C10000005',</v>
       </c>
     </row>
     <row r="6" spans="3:13">
-      <c r="C6" s="15" t="s">
-        <v>17</v>
+      <c r="C6" s="10" t="s">
+        <v>280</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>CD_FORNECEDOR,</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>42</v>
+        <v>CD_ITEM,</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" si="1"/>
-        <v>'R20000020',</v>
+        <v>'C10000006',</v>
       </c>
     </row>
     <row r="7" spans="3:13">
-      <c r="C7" s="15" t="s">
-        <v>108</v>
+      <c r="C7" s="10" t="s">
+        <v>291</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>CD_SITUACAO_PEDIDO,</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>43</v>
+        <v>DS_OBSERVACAO_ITEM,</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>157</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" si="1"/>
-        <v>'R20000021',</v>
+        <v>'C10000007',</v>
       </c>
     </row>
     <row r="8" spans="3:13">
-      <c r="C8" s="15" t="s">
-        <v>106</v>
+      <c r="C8" s="10" t="s">
+        <v>282</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>IN_APROVADO,</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>45</v>
+        <v>QT_PEDIDO,</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" si="1"/>
-        <v>'R00000009',</v>
+        <v>'C10000008',</v>
       </c>
     </row>
     <row r="9" spans="3:13">
-      <c r="C9" s="15" t="s">
-        <v>20</v>
+      <c r="C9" s="10" t="s">
+        <v>281</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>CD_CONDICAO_PAGAMENTO,</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>93</v>
+        <v>CD_UNIDADE_MEDIDA,</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>339</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" si="1"/>
-        <v>'R20000106',</v>
+        <v>'C20001859',</v>
       </c>
     </row>
     <row r="10" spans="3:13">
-      <c r="C10" s="15" t="s">
-        <v>113</v>
+      <c r="C10" s="10" t="s">
+        <v>284</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>CD_TIPO_CADASTRO,</v>
+        <v>VL_UNITARIO_ATUAL_ITEM,</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" si="1"/>
@@ -3334,15 +4723,15 @@
       </c>
     </row>
     <row r="11" spans="3:13">
-      <c r="C11" s="15" t="s">
-        <v>115</v>
+      <c r="C11" s="10" t="s">
+        <v>283</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>IN_LIQUIDACAO_AUTOMATICA,</v>
+        <v>VL_UNITARIO_ORIGINAL_ITEM,</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" si="1"/>
@@ -3350,15 +4739,15 @@
       </c>
     </row>
     <row r="12" spans="3:13">
-      <c r="C12" s="15" t="s">
-        <v>102</v>
+      <c r="C12" s="10" t="s">
+        <v>285</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>CD_TIPO_ATENDIMENTO,</v>
+        <v>QT_ENTREGUE,</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" si="1"/>
@@ -3366,210 +4755,190 @@
       </c>
     </row>
     <row r="13" spans="3:13">
-      <c r="C13" s="15" t="s">
-        <v>9</v>
+      <c r="C13" s="10" t="s">
+        <v>288</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>CD_UNIDADE_EMPRESARIAL,</v>
+        <v>QT_LIQUIDADA,</v>
       </c>
     </row>
     <row r="14" spans="3:13">
-      <c r="C14" s="15" t="s">
-        <v>8</v>
+      <c r="C14" s="10" t="s">
+        <v>289</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>CD_FILIAL,</v>
+        <v>QT_CANCELADA,</v>
       </c>
     </row>
     <row r="15" spans="3:13">
-      <c r="C15" s="15" t="s">
-        <v>116</v>
+      <c r="C15" s="10" t="s">
+        <v>286</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>CD_TIPO_ORDEM_COMPRA,</v>
+        <v>DT_ENTREGA,</v>
       </c>
     </row>
     <row r="16" spans="3:13">
-      <c r="C16" s="15" t="s">
-        <v>103</v>
+      <c r="C16" s="10" t="s">
+        <v>287</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>IN_CONSUMO,</v>
+        <v>QT_ENTREGUE_EXCESSO,</v>
       </c>
     </row>
     <row r="17" spans="3:6">
-      <c r="C17" s="15" t="s">
-        <v>35</v>
+      <c r="C17" s="10" t="s">
+        <v>290</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>CD_TIPO_FRETE,</v>
+        <v>CD_STATUS_ITEM,</v>
       </c>
     </row>
     <row r="18" spans="3:6">
-      <c r="C18" s="15" t="s">
-        <v>118</v>
+      <c r="C18" s="10" t="s">
+        <v>292</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>CD_TIPO_DOCUMENTO_FISCAL,</v>
+        <v>VL_PERCENTUAL_DESCONTO,</v>
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="C19" s="15" t="s">
-        <v>31</v>
+      <c r="C19" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>CD_TIPO_NF,</v>
+        <v>VL_FRETE,</v>
       </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="C20" s="15" t="s">
-        <v>117</v>
+      <c r="C20" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>CD_CONTRATO_VPC,</v>
+        <v>VL_SEGURO,</v>
       </c>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="15" t="s">
-        <v>101</v>
+      <c r="C21" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>VL_SALDO_PEC,</v>
+        <v>VL_FINANCEIRO,</v>
       </c>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="15" t="s">
-        <v>119</v>
+      <c r="C22" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>VL_TOTAL_MERCADORIA,</v>
+        <v>CD_NATUREZA_OPERACAO,</v>
       </c>
     </row>
     <row r="23" spans="3:6">
-      <c r="C23" s="15" t="s">
-        <v>120</v>
+      <c r="C23" s="10" t="s">
+        <v>293</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>DT_CRIACAO,</v>
+        <v>CD_ITEM_KIT,</v>
       </c>
     </row>
     <row r="24" spans="3:6">
-      <c r="C24" s="15" t="s">
-        <v>110</v>
+      <c r="C24" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>DS_USUARIO_GERACAO_PEDIDO,</v>
+        <v>DT_ATUALIZACAO,</v>
       </c>
     </row>
     <row r="25" spans="3:6">
-      <c r="C25" s="15" t="s">
-        <v>109</v>
+      <c r="C25" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>DT_SITUACAO_PEDIDO,</v>
+        <v>SQ_NATUREZA_OPERACAO,</v>
       </c>
     </row>
     <row r="26" spans="3:6">
-      <c r="C26" s="15" t="s">
-        <v>107</v>
-      </c>
+      <c r="C26" s="10"/>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>DT_APROVACAO_PEDIDO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="27" spans="3:6">
-      <c r="C27" s="15" t="s">
-        <v>105</v>
-      </c>
+      <c r="C27" s="10"/>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>DS_USUARIO_APROVACAO_PEDIDO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="28" spans="3:6">
-      <c r="C28" s="15" t="s">
-        <v>32</v>
-      </c>
+      <c r="C28" s="10"/>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>CD_NATUREZA_OPERACAO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="29" spans="3:6">
-      <c r="C29" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="C29" s="10"/>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>SQ_NATUREZA_OPERACAO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="30" spans="3:6">
-      <c r="C30" s="15" t="s">
-        <v>111</v>
-      </c>
+      <c r="C30" s="10"/>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>DS_OBSERVACAO_PEDIDO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="31" spans="3:6">
-      <c r="C31" s="15" t="s">
-        <v>112</v>
-      </c>
+      <c r="C31" s="10"/>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>CD_DEPARTAMENTO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="32" spans="3:6">
-      <c r="C32" s="15" t="s">
-        <v>13</v>
-      </c>
+      <c r="C32" s="10"/>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>VL_FRETE,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="33" spans="3:6">
-      <c r="C33" s="15" t="s">
-        <v>19</v>
-      </c>
+      <c r="C33" s="10"/>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>VL_SEGURO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="34" spans="3:6">
-      <c r="C34" s="15" t="s">
-        <v>114</v>
-      </c>
+      <c r="C34" s="10"/>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>VL_FINANCEIRO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="35" spans="3:6">
-      <c r="C35" s="15" t="s">
-        <v>34</v>
-      </c>
+      <c r="C35" s="10"/>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>DT_ATUALIZACAO,</v>
+        <v>,</v>
       </c>
     </row>
     <row r="36" spans="3:6">

</xml_diff>